<commit_message>
Tests tst_csv2ts, tst_ts2csv, ts2_xlx run smooth; tst_xlsx needs fixes
</commit_message>
<xml_diff>
--- a/tests/files/scenario_after_version_4_5_0.xlsx
+++ b/tests/files/scenario_after_version_4_5_0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>TsVersion</t>
   </si>
@@ -22,15 +22,42 @@
     <t>2.1</t>
   </si>
   <si>
+    <t>sourcelanguage</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
     <t>Context</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
     <t>Translation</t>
   </si>
   <si>
+    <t>TranslationType</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>extracomment</t>
+  </si>
+  <si>
+    <t>translatorcomment</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
@@ -43,22 +70,49 @@
     <t/>
   </si>
   <si>
+    <t>unfinished</t>
+  </si>
+  <si>
+    <t>my comment</t>
+  </si>
+  <si>
     <t>../src/app/qml/MenuBar.qml - 17</t>
   </si>
   <si>
+    <t>1abc</t>
+  </si>
+  <si>
     <t>map</t>
   </si>
   <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>vanished</t>
+  </si>
+  <si>
+    <t>extra comment test</t>
+  </si>
+  <si>
     <t>../src/app/qml/MenuBar.qml - 28</t>
   </si>
   <si>
     <t>cam</t>
   </si>
   <si>
+    <t>whichever</t>
+  </si>
+  <si>
+    <t>obsolete</t>
+  </si>
+  <si>
     <t>../src/app/qml/MenuBar.qml - 43</t>
   </si>
   <si>
     <t>checklist</t>
+  </si>
+  <si>
+    <t>mytranslation</t>
   </si>
   <si>
     <t>../src/app/qml/MenuBar.qml - 58</t>
@@ -389,23 +443,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -418,47 +484,110 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B4"/>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B6"/>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>15</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>